<commit_message>
Excel2Json for registering voters
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -20,21 +20,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">level</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">lrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gradeLevel</t>
   </si>
   <si>
     <t xml:space="preserve">section</t>
   </si>
   <si>
-    <t xml:space="preserve">adem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cpa</t>
+    <t xml:space="preserve">Abdul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kribek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clementine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secion Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section C</t>
   </si>
 </sst>
 </file>
@@ -49,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,37 +185,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>0</v>
+      <c r="A2" s="0" t="n">
+        <v>106167030444</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="0" t="n">
+        <v>103243766545</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>106672080991</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>113344505123</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>101010111001</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>